<commit_message>
minor improvement, avoid to use hard-coded relationId
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE01B21-903B-4477-ADEB-473770427ABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C75A484-5E4D-41ED-8B0A-6ED38BD9ECD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,10 +32,19 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={85637300-450C-4380-BF4A-D6C68B5985E0}</author>
     <author>tc={74640F05-764D-4B33-BCC4-F16AE36A81EB}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{74640F05-764D-4B33-BCC4-F16AE36A81EB}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{85637300-450C-4380-BF4A-D6C68B5985E0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If this field is set, test case will use its value to get a list of relations, then pick up the id of the 1st relation as the relationId value to be test and the input parameter "relationId" will be ignored.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{74640F05-764D-4B33-BCC4-F16AE36A81EB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -48,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
   <si>
     <t>OK</t>
   </si>
@@ -246,13 +255,19 @@
   </si>
   <si>
     <t>good request, get all relations</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>is_instance_of</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +287,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -617,7 +638,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2021-01-18T04:34:12.95" personId="{DC27ECC5-F7F2-49C3-B546-5535111A3B3F}" id="{74640F05-764D-4B33-BCC4-F16AE36A81EB}">
+  <threadedComment ref="C1" dT="2021-01-18T06:55:27.50" personId="{DC27ECC5-F7F2-49C3-B546-5535111A3B3F}" id="{85637300-450C-4380-BF4A-D6C68B5985E0}">
+    <text>If this field is set, test case will use its value to get a list of relations, then pick up the id of the 1st relation as the relationId value to be test and the input parameter "relationId" will be ignored.</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2021-01-18T04:34:12.95" personId="{DC27ECC5-F7F2-49C3-B546-5535111A3B3F}" id="{74640F05-764D-4B33-BCC4-F16AE36A81EB}">
     <text>Note: use the same id may lead to test fail in different environments, as the ids in dev/test/prod environment are different!</text>
   </threadedComment>
 </ThreadedComments>
@@ -1261,21 +1285,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="12.54296875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="3" width="30.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1283,95 +1307,106 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="6">
         <v>25018</v>
       </c>
-      <c r="D2" s="6">
-        <v>200</v>
-      </c>
       <c r="E2" s="6">
         <v>200</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="6">
+        <v>200</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="6">
         <v>31233</v>
       </c>
-      <c r="D3" s="6">
-        <v>200</v>
-      </c>
       <c r="E3" s="6">
         <v>200</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="6">
+        <v>200</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>400</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>103000</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2">
         <v>9999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>500</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add test execution functions
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF7A62-E1FD-4BBE-8863-0E2704D35B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC4ECE-5DC6-468B-AA04-BB90B6302E20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createEntityInDomain" sheetId="5" r:id="rId1"/>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C10F18-6774-4DA2-A97E-6CA070C2B102}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3">
-        <v>1234</v>
+        <v>123456789</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -1001,7 +1001,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="5">
-        <v>9999</v>
+        <v>999999</v>
       </c>
       <c r="F4" s="2">
         <v>200</v>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="2">
-        <v>9999</v>
+        <v>999999</v>
       </c>
       <c r="E5" s="2">
         <v>500</v>

</xml_diff>

<commit_message>
fix entity management test fails due to feature update
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC4ECE-5DC6-468B-AA04-BB90B6302E20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DF413E-17EE-43C2-B0B9-9F7788671F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="createEntityInDomain" sheetId="5" r:id="rId1"/>
+    <sheet name="createEntity" sheetId="5" r:id="rId1"/>
     <sheet name="updateEntity" sheetId="3" r:id="rId2"/>
     <sheet name="deleteEntity" sheetId="4" r:id="rId3"/>
     <sheet name="getEntityById" sheetId="2" r:id="rId4"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>OK</t>
   </si>
@@ -80,12 +80,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -95,15 +89,9 @@
     <t>body</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>abcde123</t>
   </si>
   <si>
-    <t>id format invalid</t>
-  </si>
-  <si>
     <t>bad request, entity id not a number</t>
   </si>
   <si>
@@ -119,30 +107,15 @@
     <t>Device_Modelqwerqwr3r23rwer*()(!@#$%%^&amp;*</t>
   </si>
   <si>
-    <t>no valid label</t>
-  </si>
-  <si>
     <t>bad request, body is empty</t>
   </si>
   <si>
     <t>{}</t>
   </si>
   <si>
-    <t>same entity</t>
-  </si>
-  <si>
-    <t>No message available</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>entity id invalid</t>
   </si>
   <si>
-    <t>id not exist</t>
-  </si>
-  <si>
     <t>labels</t>
   </si>
   <si>
@@ -164,9 +137,6 @@
     <t>relationId</t>
   </si>
   <si>
-    <t>getRelationById.relationId: id format invalid</t>
-  </si>
-  <si>
     <t>iEMS-Entity-mgmt-Test-1</t>
   </si>
   <si>
@@ -185,9 +155,6 @@
     <t>iEMS-Entity-mgmt-Test-2</t>
   </si>
   <si>
-    <t>{"id":"41","label":"Device","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
-  </si>
-  <si>
     <t>iEMS-Entity-mgmt-Test-9-var1</t>
   </si>
   <si>
@@ -197,9 +164,6 @@
     <t>iEMS-Entity-mgmt-Test-9-var3</t>
   </si>
   <si>
-    <t>{"id":"abcde","label":"Device","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
-  </si>
-  <si>
     <t>iEMS-Entity-mgmt-Test-3</t>
   </si>
   <si>
@@ -257,13 +221,43 @@
     <t>is_instance_of</t>
   </si>
   <si>
-    <t>{"id":"99999","label":"Device","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
-  </si>
-  <si>
     <t>bad request, relationId not exist</t>
   </si>
   <si>
     <t>bad request, relationId is invalid</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>same label</t>
+  </si>
+  <si>
+    <t>label invalid</t>
+  </si>
+  <si>
+    <t>format invalid</t>
+  </si>
+  <si>
+    <t>entity doesn't exist</t>
+  </si>
+  <si>
+    <t>is empty</t>
+  </si>
+  <si>
+    <t>not exist</t>
+  </si>
+  <si>
+    <t>relation doesn't exist</t>
+  </si>
+  <si>
+    <t>{"id":"41","label":"testEntity1","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
+  </si>
+  <si>
+    <t>{"id":"99999","label":"testEntity1","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
+  </si>
+  <si>
+    <t>{"id":"abcde","label":"testEntity1","properties":{"metadata_node_type":"entity","metadata_node_domain":"iEMS","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"iEMS"}</t>
   </si>
 </sst>
 </file>
@@ -649,7 +643,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -662,16 +656,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -685,13 +679,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -708,13 +702,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
@@ -723,24 +717,24 @@
         <v>400</v>
       </c>
       <c r="F3" s="2">
-        <v>10300</v>
+        <v>103000</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>400</v>
@@ -749,7 +743,7 @@
         <v>103000</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +758,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -778,19 +772,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
@@ -804,19 +798,19 @@
     </row>
     <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -830,59 +824,59 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2">
-        <v>500</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>400</v>
+      </c>
+      <c r="G3" s="2">
+        <v>103000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="2">
-        <v>200</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>400</v>
+      </c>
+      <c r="G4" s="2">
+        <v>103000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2">
         <v>400</v>
@@ -891,7 +885,7 @@
         <v>103000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -905,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C10F18-6774-4DA2-A97E-6CA070C2B102}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -919,16 +913,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
@@ -945,13 +939,13 @@
     </row>
     <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -963,23 +957,23 @@
         <v>200</v>
       </c>
       <c r="G2" s="2">
+        <v>200</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -988,15 +982,15 @@
         <v>103000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1007,10 +1001,10 @@
         <v>200</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>103000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1024,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68ECACFD-75AA-40A8-8500-FACA5E36F33B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1038,16 +1032,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
@@ -1064,13 +1058,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -1090,15 +1084,15 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -1107,29 +1101,29 @@
         <v>103000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="5">
-        <v>99999</v>
+        <v>999999</v>
       </c>
       <c r="F4" s="2">
-        <v>500</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>200</v>
+      </c>
+      <c r="G4" s="2">
+        <v>103000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1157,13 +1151,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
@@ -1177,10 +1171,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6">
@@ -1195,13 +1189,13 @@
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -1215,13 +1209,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -1235,13 +1229,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>200</v>
@@ -1255,13 +1249,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2">
         <v>200</v>
@@ -1285,7 +1279,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1298,16 +1292,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1321,13 +1315,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6">
         <v>25018</v>
@@ -1344,13 +1338,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D3" s="6">
         <v>31233</v>
@@ -1367,14 +1361,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
         <v>400</v>
@@ -1383,28 +1377,28 @@
         <v>103000</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="2">
         <v>999999</v>
       </c>
       <c r="E5" s="2">
-        <v>500</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>200</v>
+      </c>
+      <c r="F5" s="2">
+        <v>103000</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cases of iems
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EF32D1-8B2C-42C5-92D6-668B8025C810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEFBA33-60BE-4B3F-8CEB-54C64E0996D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="391">
   <si>
     <t>testEntity1</t>
   </si>
@@ -714,9 +714,6 @@
   </si>
   <si>
     <t>NOT_EXIST</t>
-  </si>
-  <si>
-    <t>java.util.concurrent.CompletionException: org.apache.tinkerpop.gremlin.driver.exception.ResponseException</t>
   </si>
   <si>
     <t>[
@@ -3860,6 +3857,9 @@
   </si>
   <si>
     <t>Edge [[abcde123]] not exist!</t>
+  </si>
+  <si>
+    <t>Entity [[abcde123]] not exist!</t>
   </si>
 </sst>
 </file>
@@ -4312,21 +4312,21 @@
         <v>2</v>
       </c>
       <c r="AA1" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="21:28" ht="409.6">
       <c r="U2" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="V2" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="V2" s="11" t="s">
-        <v>233</v>
-      </c>
       <c r="W2" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="X2" s="12" t="s">
         <v>35</v>
@@ -4342,13 +4342,13 @@
     </row>
     <row r="3" spans="21:28" ht="409.6">
       <c r="U3" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="V3" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>236</v>
       </c>
       <c r="X3" s="5">
         <v>200</v>
@@ -4357,22 +4357,22 @@
         <v>100000</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA3" s="14"/>
       <c r="AB3" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="21:28" ht="409.6">
       <c r="U4" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="V4" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="W4" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="W4" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="X4" s="5">
         <v>200</v>
@@ -4381,22 +4381,22 @@
         <v>100000</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA4" s="14"/>
       <c r="AB4" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="21:28" ht="409.6">
       <c r="U5" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="V5" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="W5" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="W5" s="14" t="s">
-        <v>244</v>
       </c>
       <c r="X5" s="5">
         <v>200</v>
@@ -4405,22 +4405,22 @@
         <v>100000</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA5" s="5"/>
       <c r="AB5" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="21:28" ht="409.6">
       <c r="U6" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="V6" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="W6" s="14" t="s">
-        <v>248</v>
       </c>
       <c r="X6" s="5">
         <v>200</v>
@@ -4429,20 +4429,20 @@
         <v>100000</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
     <row r="7" spans="21:28" ht="409.6">
       <c r="U7" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="V7" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="V7" s="14" t="s">
+      <c r="W7" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="W7" s="14" t="s">
-        <v>251</v>
       </c>
       <c r="X7" s="5">
         <v>200</v>
@@ -4451,22 +4451,22 @@
         <v>100000</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="21:28" ht="409.6">
       <c r="U8" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="V8" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="W8" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="W8" s="14" t="s">
-        <v>255</v>
       </c>
       <c r="X8" s="5">
         <v>200</v>
@@ -4475,20 +4475,20 @@
         <v>100000</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
     </row>
     <row r="9" spans="21:28" ht="409.6">
       <c r="U9" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="V9" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="W9" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="W9" s="14" t="s">
-        <v>258</v>
       </c>
       <c r="X9" s="5">
         <v>200</v>
@@ -4497,7 +4497,7 @@
         <v>100000</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5" t="s">
@@ -4506,13 +4506,13 @@
     </row>
     <row r="10" spans="21:28" ht="409.6">
       <c r="U10" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="V10" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="W10" s="14" t="s">
         <v>260</v>
-      </c>
-      <c r="W10" s="14" t="s">
-        <v>261</v>
       </c>
       <c r="X10" s="5">
         <v>200</v>
@@ -4521,20 +4521,20 @@
         <v>100000</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
     </row>
     <row r="11" spans="21:28" ht="409.6">
       <c r="U11" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="V11" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="V11" s="14" t="s">
+      <c r="W11" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="W11" s="14" t="s">
-        <v>264</v>
       </c>
       <c r="X11" s="5">
         <v>200</v>
@@ -4543,20 +4543,20 @@
         <v>100000</v>
       </c>
       <c r="Z11" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
     </row>
     <row r="12" spans="21:28" ht="409.6">
       <c r="U12" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="V12" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="V12" s="14" t="s">
+      <c r="W12" s="14" t="s">
         <v>266</v>
-      </c>
-      <c r="W12" s="14" t="s">
-        <v>267</v>
       </c>
       <c r="X12" s="5">
         <v>200</v>
@@ -4565,22 +4565,22 @@
         <v>100000</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="21:28" ht="409.6">
       <c r="U13" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="V13" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="V13" s="14" t="s">
+      <c r="W13" s="14" t="s">
         <v>270</v>
-      </c>
-      <c r="W13" s="14" t="s">
-        <v>271</v>
       </c>
       <c r="X13" s="5">
         <v>200</v>
@@ -4589,22 +4589,22 @@
         <v>100000</v>
       </c>
       <c r="Z13" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="21:28" ht="409.6">
       <c r="U14" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="V14" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="V14" s="14" t="s">
+      <c r="W14" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="W14" s="14" t="s">
-        <v>275</v>
       </c>
       <c r="X14" s="5">
         <v>200</v>
@@ -4613,22 +4613,22 @@
         <v>100000</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="21:28" ht="409.6">
       <c r="U15" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="V15" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="V15" s="14" t="s">
+      <c r="W15" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="W15" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="X15" s="5">
         <v>200</v>
@@ -4637,22 +4637,22 @@
         <v>100000</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="21:28" ht="409.6">
       <c r="U16" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="V16" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="V16" s="14" t="s">
+      <c r="W16" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="W16" s="14" t="s">
-        <v>281</v>
       </c>
       <c r="X16" s="5">
         <v>200</v>
@@ -4661,20 +4661,20 @@
         <v>100000</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
     </row>
     <row r="17" spans="21:28" ht="409.6">
       <c r="U17" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="V17" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="W17" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="W17" s="14" t="s">
-        <v>284</v>
       </c>
       <c r="X17" s="5">
         <v>200</v>
@@ -4683,20 +4683,20 @@
         <v>100000</v>
       </c>
       <c r="Z17" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
     </row>
     <row r="18" spans="21:28" ht="409.6">
       <c r="U18" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="V18" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="V18" s="14" t="s">
+      <c r="W18" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="W18" s="14" t="s">
-        <v>287</v>
       </c>
       <c r="X18" s="5">
         <v>200</v>
@@ -4705,7 +4705,7 @@
         <v>100000</v>
       </c>
       <c r="Z18" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5" t="s">
@@ -4714,13 +4714,13 @@
     </row>
     <row r="19" spans="21:28" ht="409.6">
       <c r="U19" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="V19" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="V19" s="14" t="s">
+      <c r="W19" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="W19" s="14" t="s">
-        <v>290</v>
       </c>
       <c r="X19" s="5">
         <v>200</v>
@@ -4729,7 +4729,7 @@
         <v>100000</v>
       </c>
       <c r="Z19" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5" t="s">
@@ -4738,13 +4738,13 @@
     </row>
     <row r="20" spans="21:28" ht="409.6">
       <c r="U20" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="V20" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="V20" s="14" t="s">
+      <c r="W20" s="14" t="s">
         <v>292</v>
-      </c>
-      <c r="W20" s="14" t="s">
-        <v>293</v>
       </c>
       <c r="X20" s="5">
         <v>200</v>
@@ -4753,7 +4753,7 @@
         <v>100000</v>
       </c>
       <c r="Z20" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA20" s="5"/>
       <c r="AB20" s="5" t="s">
@@ -4762,13 +4762,13 @@
     </row>
     <row r="21" spans="21:28" ht="409.6">
       <c r="U21" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="V21" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="V21" s="14" t="s">
+      <c r="W21" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="W21" s="14" t="s">
-        <v>296</v>
       </c>
       <c r="X21" s="5">
         <v>200</v>
@@ -4777,22 +4777,22 @@
         <v>100000</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA21" s="5"/>
       <c r="AB21" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="21:28" ht="409.6">
       <c r="U22" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="V22" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="V22" s="14" t="s">
+      <c r="W22" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="W22" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="X22" s="5">
         <v>200</v>
@@ -4801,22 +4801,22 @@
         <v>100000</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="21:28" ht="409.6">
       <c r="U23" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="V23" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="W23" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="W23" s="14" t="s">
-        <v>304</v>
       </c>
       <c r="X23" s="5">
         <v>200</v>
@@ -4825,22 +4825,22 @@
         <v>100000</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="21:28" ht="409.6">
       <c r="U24" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="V24" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="V24" s="14" t="s">
+      <c r="W24" s="20" t="s">
         <v>306</v>
-      </c>
-      <c r="W24" s="20" t="s">
-        <v>307</v>
       </c>
       <c r="X24" s="5">
         <v>200</v>
@@ -4849,21 +4849,21 @@
         <v>100000</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AB24" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="21:28" ht="409.6">
       <c r="U25" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="V25" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="V25" s="14" t="s">
+      <c r="W25" s="20" t="s">
         <v>310</v>
-      </c>
-      <c r="W25" s="20" t="s">
-        <v>311</v>
       </c>
       <c r="X25" s="5">
         <v>200</v>
@@ -4872,21 +4872,21 @@
         <v>100000</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AB25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="21:28" ht="409.6">
       <c r="U26" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="V26" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="W26" s="20" t="s">
         <v>314</v>
-      </c>
-      <c r="W26" s="20" t="s">
-        <v>315</v>
       </c>
       <c r="X26" s="5">
         <v>200</v>
@@ -4895,18 +4895,18 @@
         <v>100000</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="21:28" ht="409.6">
       <c r="U27" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="V27" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="V27" s="14" t="s">
+      <c r="W27" s="20" t="s">
         <v>317</v>
-      </c>
-      <c r="W27" s="20" t="s">
-        <v>318</v>
       </c>
       <c r="X27" s="5">
         <v>200</v>
@@ -4915,18 +4915,18 @@
         <v>100000</v>
       </c>
       <c r="Z27" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="21:28" ht="409.6">
       <c r="U28" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="V28" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="V28" s="14" t="s">
+      <c r="W28" s="20" t="s">
         <v>320</v>
-      </c>
-      <c r="W28" s="20" t="s">
-        <v>321</v>
       </c>
       <c r="X28" s="5">
         <v>200</v>
@@ -4935,7 +4935,7 @@
         <v>100000</v>
       </c>
       <c r="Z28" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5006,13 +5006,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -5034,11 +5034,11 @@
         <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E3" s="8">
         <v>400</v>
@@ -5056,11 +5056,11 @@
         <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="8">
         <v>400</v>
@@ -5078,11 +5078,11 @@
         <v>62</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5" s="8">
         <v>400</v>
@@ -5100,11 +5100,11 @@
         <v>63</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="8">
         <v>400</v>
@@ -5122,11 +5122,11 @@
         <v>64</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="8">
         <v>400</v>
@@ -5144,11 +5144,11 @@
         <v>65</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E8" s="8">
         <v>400</v>
@@ -5162,7 +5162,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="111" customHeight="1">
@@ -5170,11 +5170,11 @@
         <v>66</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="8">
         <v>400</v>
@@ -5188,7 +5188,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="111" customHeight="1">
@@ -5196,11 +5196,11 @@
         <v>67</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="8">
         <v>400</v>
@@ -5214,19 +5214,19 @@
       <c r="H10" s="12"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="111" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E11" s="8">
         <v>400</v>
@@ -5240,19 +5240,19 @@
       <c r="H11" s="12"/>
       <c r="I11" s="6"/>
       <c r="J11" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="111" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="8">
         <v>400</v>
@@ -5271,14 +5271,14 @@
     </row>
     <row r="13" spans="1:10" ht="111" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E13" s="8">
         <v>400</v>
@@ -5297,14 +5297,14 @@
     </row>
     <row r="14" spans="1:10" ht="111" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="8">
         <v>400</v>
@@ -5318,19 +5318,19 @@
       <c r="H14" s="12"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="111" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E15" s="8">
         <v>400</v>
@@ -5349,14 +5349,14 @@
     </row>
     <row r="16" spans="1:10" ht="111" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" s="8">
         <v>400</v>
@@ -5375,14 +5375,14 @@
     </row>
     <row r="17" spans="1:10" ht="111" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E17" s="8">
         <v>400</v>
@@ -5401,14 +5401,14 @@
     </row>
     <row r="18" spans="1:10" ht="111" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" s="8">
         <v>400</v>
@@ -5427,14 +5427,14 @@
     </row>
     <row r="19" spans="1:10" ht="111" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="8">
         <v>400</v>
@@ -5453,14 +5453,14 @@
     </row>
     <row r="20" spans="1:10" ht="111" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E20" s="8">
         <v>400</v>
@@ -5479,14 +5479,14 @@
     </row>
     <row r="21" spans="1:10" ht="111" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E21" s="8">
         <v>400</v>
@@ -5505,14 +5505,14 @@
     </row>
     <row r="22" spans="1:10" ht="111" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E22" s="8">
         <v>400</v>
@@ -5531,14 +5531,14 @@
     </row>
     <row r="23" spans="1:10" ht="111" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23" s="8">
         <v>400</v>
@@ -5557,14 +5557,14 @@
     </row>
     <row r="24" spans="1:10" ht="111" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E24" s="8">
         <v>400</v>
@@ -5578,19 +5578,19 @@
       <c r="H24" s="12"/>
       <c r="I24" s="6"/>
       <c r="J24" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="111" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E25" s="8">
         <v>200</v>
@@ -5602,7 +5602,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
@@ -5618,7 +5618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5FE0E-8788-403D-8502-6CD26A71119B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -5678,16 +5678,16 @@
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="F2" s="12">
         <v>200</v>
@@ -5732,12 +5732,12 @@
         <v>30</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>85</v>
@@ -5759,12 +5759,12 @@
         <v>31</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>85</v>
@@ -5773,7 +5773,7 @@
         <v>86</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="6"/>
@@ -5788,10 +5788,10 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="F6" s="12">
         <v>200</v>
@@ -5874,10 +5874,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>71</v>
@@ -5915,7 +5915,7 @@
         <v>101400</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="27.6">
@@ -5938,7 +5938,7 @@
         <v>101400</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -6033,7 +6033,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -6131,10 +6131,10 @@
         <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>71</v>
@@ -6161,10 +6161,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>58</v>
@@ -6213,7 +6213,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="10"/>
       <c r="F5" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G5" s="10">
         <v>200</v>
@@ -6259,10 +6259,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>324</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>4</v>
@@ -6276,19 +6276,19 @@
     </row>
     <row r="2" spans="1:8" ht="409.6">
       <c r="A2" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>35</v>
@@ -6344,21 +6344,21 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.6">
       <c r="A2" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>35</v>
@@ -6374,13 +6374,13 @@
     </row>
     <row r="3" spans="1:8" ht="409.6">
       <c r="A3" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -6389,21 +6389,21 @@
         <v>100000</v>
       </c>
       <c r="F3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" t="s">
         <v>237</v>
-      </c>
-      <c r="H3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="409.6">
       <c r="A4" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D4">
         <v>200</v>
@@ -6412,21 +6412,21 @@
         <v>100000</v>
       </c>
       <c r="F4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H4" t="s">
         <v>237</v>
-      </c>
-      <c r="H4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="216">
       <c r="A5" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>346</v>
       </c>
       <c r="D5">
         <v>200</v>
@@ -6435,21 +6435,21 @@
         <v>100000</v>
       </c>
       <c r="F5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="244.8">
       <c r="A6" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>348</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>349</v>
       </c>
       <c r="D6">
         <v>200</v>
@@ -6458,21 +6458,21 @@
         <v>100000</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="409.6">
       <c r="A7" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>350</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>351</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -6481,21 +6481,21 @@
         <v>100000</v>
       </c>
       <c r="F7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.6">
       <c r="A8" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D8">
         <v>200</v>
@@ -6504,18 +6504,18 @@
         <v>100000</v>
       </c>
       <c r="F8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="409.6">
       <c r="A9" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -6524,18 +6524,18 @@
         <v>100000</v>
       </c>
       <c r="F9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="409.6">
       <c r="A10" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D10">
         <v>200</v>
@@ -6544,7 +6544,7 @@
         <v>100000</v>
       </c>
       <c r="F10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H10" t="s">
         <v>109</v>
@@ -6552,13 +6552,13 @@
     </row>
     <row r="11" spans="1:8" ht="409.6">
       <c r="A11" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -6567,21 +6567,21 @@
         <v>100000</v>
       </c>
       <c r="F11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="409.6">
       <c r="A12" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>355</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>356</v>
       </c>
       <c r="D12">
         <v>200</v>
@@ -6590,21 +6590,21 @@
         <v>100000</v>
       </c>
       <c r="F12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="409.6">
       <c r="A13" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D13">
         <v>200</v>
@@ -6613,7 +6613,7 @@
         <v>100000</v>
       </c>
       <c r="F13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H13" t="s">
         <v>102</v>
@@ -6621,13 +6621,13 @@
     </row>
     <row r="14" spans="1:8" ht="409.6">
       <c r="A14" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D14">
         <v>200</v>
@@ -6636,18 +6636,18 @@
         <v>100000</v>
       </c>
       <c r="F14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.6">
       <c r="A15" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D15">
         <v>200</v>
@@ -6656,18 +6656,18 @@
         <v>100000</v>
       </c>
       <c r="F15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="409.6">
       <c r="A16" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D16">
         <v>200</v>
@@ -6676,21 +6676,21 @@
         <v>100000</v>
       </c>
       <c r="F16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="409.6">
       <c r="A17" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D17">
         <v>200</v>
@@ -6699,7 +6699,7 @@
         <v>100000</v>
       </c>
       <c r="F17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H17" t="s">
         <v>102</v>
@@ -6707,13 +6707,13 @@
     </row>
     <row r="18" spans="1:8" ht="409.6">
       <c r="A18" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D18">
         <v>200</v>
@@ -6722,7 +6722,7 @@
         <v>100000</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H18" t="s">
         <v>109</v>
@@ -6730,13 +6730,13 @@
     </row>
     <row r="19" spans="1:8" ht="409.6">
       <c r="A19" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D19">
         <v>200</v>
@@ -6745,21 +6745,21 @@
         <v>100000</v>
       </c>
       <c r="F19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="409.6">
       <c r="A20" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D20">
         <v>200</v>
@@ -6768,21 +6768,21 @@
         <v>100000</v>
       </c>
       <c r="F20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="409.6">
       <c r="A21" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>365</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>366</v>
       </c>
       <c r="D21">
         <v>200</v>
@@ -6791,21 +6791,21 @@
         <v>100000</v>
       </c>
       <c r="F21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="409.6">
       <c r="A22" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D22">
         <v>200</v>
@@ -6814,21 +6814,21 @@
         <v>100000</v>
       </c>
       <c r="F22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="216">
       <c r="A23" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B23" t="s">
+        <v>367</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>369</v>
       </c>
       <c r="D23">
         <v>200</v>
@@ -6837,7 +6837,7 @@
         <v>100000</v>
       </c>
       <c r="F23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H23" t="s">
         <v>109</v>
@@ -6932,7 +6932,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>96</v>
@@ -6953,7 +6953,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>88</v>
@@ -6974,7 +6974,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>97</v>
@@ -7070,7 +7070,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>99</v>
@@ -7095,7 +7095,7 @@
         <v>92</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>105</v>
@@ -7237,7 +7237,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="106.2" customHeight="1">
@@ -7348,7 +7348,7 @@
         <v>54</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>35</v>
@@ -7376,8 +7376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B97966-D445-41D3-A12C-5E1768A05176}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -7521,7 +7521,7 @@
         <v>36</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>16</v>
+        <v>388</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="6"/>
@@ -7535,10 +7535,10 @@
         <v>137</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="E6" s="12">
         <v>200</v>
@@ -7567,7 +7567,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -7635,7 +7635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="69">
+    <row r="3" spans="1:8" ht="27.6">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>101400</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>141</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -7676,7 +7676,7 @@
         <v>101400</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -7771,7 +7771,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -7915,7 +7915,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -7971,7 +7971,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="10">
         <v>200</v>
@@ -7991,7 +7991,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>57</v>
@@ -8009,7 +8009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69">
+    <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
@@ -8021,14 +8021,14 @@
       <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="10">
-        <v>400</v>
+      <c r="F4" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -8041,7 +8041,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="10">
         <v>200</v>

</xml_diff>